<commit_message>
EPBDS-9041 fix casting from boxed types to primitives
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastNulls.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastNulls.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvlad\.openl-webstudio\user-workspace\admin\EPBDS-9041_18\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E27E6-658B-478B-A630-6089D6736BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object" sheetId="5" r:id="rId1"/>
     <sheet name="Array" sheetId="6" r:id="rId2"/>
+    <sheet name="Spreadsheet Default Values" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="129">
   <si>
     <t>step</t>
   </si>
@@ -140,13 +142,309 @@
   </si>
   <si>
     <t>Test arrayCastDown arrayCastDownTest</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>byte:byte</t>
+  </si>
+  <si>
+    <t>short:short</t>
+  </si>
+  <si>
+    <t>char:char</t>
+  </si>
+  <si>
+    <t>int:int</t>
+  </si>
+  <si>
+    <t>long:long</t>
+  </si>
+  <si>
+    <t>float:float</t>
+  </si>
+  <si>
+    <t>double:double</t>
+  </si>
+  <si>
+    <t>boolean:boolean</t>
+  </si>
+  <si>
+    <t>Byte:Byte</t>
+  </si>
+  <si>
+    <t>Short:Short</t>
+  </si>
+  <si>
+    <t>Integer:Integer</t>
+  </si>
+  <si>
+    <t>Long:Long</t>
+  </si>
+  <si>
+    <t>Float:Float</t>
+  </si>
+  <si>
+    <t>Double:Double</t>
+  </si>
+  <si>
+    <t>Boolean:Boolean</t>
+  </si>
+  <si>
+    <t>String:String</t>
+  </si>
+  <si>
+    <t>Character:Character</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sprDefaultValues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ()</t>
+    </r>
+  </si>
+  <si>
+    <t>_description_</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>_res_.$V$byte</t>
+  </si>
+  <si>
+    <t>_res_.$V$short</t>
+  </si>
+  <si>
+    <t>_res_.$V$char</t>
+  </si>
+  <si>
+    <t>_res_.$V$int</t>
+  </si>
+  <si>
+    <t>_res_.$V$long</t>
+  </si>
+  <si>
+    <t>_res_.$V$double</t>
+  </si>
+  <si>
+    <t>_res_.$V$boolean</t>
+  </si>
+  <si>
+    <t>_res_.$V$Byte</t>
+  </si>
+  <si>
+    <t>_res_.$V$Short</t>
+  </si>
+  <si>
+    <t>BigDecimal:BigDecimal</t>
+  </si>
+  <si>
+    <t>BigInteger:BigInteger</t>
+  </si>
+  <si>
+    <t>_res_.$V$Character</t>
+  </si>
+  <si>
+    <t>_res_.$V$Integer</t>
+  </si>
+  <si>
+    <t>_res_.$V$Long</t>
+  </si>
+  <si>
+    <t>_res_.$V$Float</t>
+  </si>
+  <si>
+    <t>_res_.$V$Double</t>
+  </si>
+  <si>
+    <t>_res_.$V$Boolean</t>
+  </si>
+  <si>
+    <t>_res_.$V$String</t>
+  </si>
+  <si>
+    <t>_res_.$V$BigDecimal</t>
+  </si>
+  <si>
+    <t>_res_.$V$BigInteger</t>
+  </si>
+  <si>
+    <t>ByteValue:ByteValue</t>
+  </si>
+  <si>
+    <t>ShortValue:ShortValue</t>
+  </si>
+  <si>
+    <t>IntValue:IntValue</t>
+  </si>
+  <si>
+    <t>LongValue:LongValue</t>
+  </si>
+  <si>
+    <t>FloatValue:FloatValue</t>
+  </si>
+  <si>
+    <t>DoubleValue:DoubleValue</t>
+  </si>
+  <si>
+    <t>StringValue:StringValue</t>
+  </si>
+  <si>
+    <t>BigDecimalValue:BigDecimalValue</t>
+  </si>
+  <si>
+    <t>BigIntegerValue:BigIntegerValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$ByteValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$ShortValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$IntValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$LongValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$FloatValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$DoubleValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$StringValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$BigDecimalValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$BigIntegerValue</t>
+  </si>
+  <si>
+    <t>_res_.$V$float</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>BigDecimal</t>
+  </si>
+  <si>
+    <t>BigInteger</t>
+  </si>
+  <si>
+    <t>ByteValue</t>
+  </si>
+  <si>
+    <t>ShortValue</t>
+  </si>
+  <si>
+    <t>IntValue</t>
+  </si>
+  <si>
+    <t>LongValue</t>
+  </si>
+  <si>
+    <t>FloatValue</t>
+  </si>
+  <si>
+    <t>DoubleValue</t>
+  </si>
+  <si>
+    <t>StringValue</t>
+  </si>
+  <si>
+    <t>BigDecimalValue</t>
+  </si>
+  <si>
+    <t>BigIntegerValue</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sprDefaultValues</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -157,16 +455,46 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,11 +502,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -192,9 +535,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -210,9 +579,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -250,7 +619,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -356,7 +725,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,28 +898,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="9" max="9" width="4.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -563,7 +932,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -578,7 +947,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -593,7 +962,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -618,29 +987,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -648,7 +1017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -656,13 +1025,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -670,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -678,13 +1047,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -692,7 +1061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -700,7 +1069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>26</v>
       </c>
@@ -708,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -716,7 +1085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -729,7 +1098,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -746,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -763,7 +1132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>36</v>
       </c>
@@ -789,4 +1158,498 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C429AF-F69B-4448-8019-867CDC5C634E}">
+  <dimension ref="B5:D71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B40:D40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>